<commit_message>
V20 - Improved data logging and added functionality to start/stop data logging as well as edit filename and output path in program.
</commit_message>
<xml_diff>
--- a/MCC-DAQ backup/temp.xlsx
+++ b/MCC-DAQ backup/temp.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,7 +434,7 @@
         <v>22.7</v>
       </c>
       <c r="D2">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
       <c r="E2">
         <v>22</v>
@@ -454,7 +454,7 @@
         <v>22.6</v>
       </c>
       <c r="D3">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
       <c r="E3">
         <v>22</v>
@@ -494,7 +494,7 @@
         <v>22.6</v>
       </c>
       <c r="D5">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
       <c r="E5">
         <v>22</v>
@@ -514,7 +514,7 @@
         <v>22.6</v>
       </c>
       <c r="D6">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
       <c r="E6">
         <v>22</v>
@@ -534,12 +534,1632 @@
         <v>22.6</v>
       </c>
       <c r="D7">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
       <c r="E7">
         <v>22</v>
       </c>
       <c r="F7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>22.5</v>
+      </c>
+      <c r="C8">
+        <v>22.6</v>
+      </c>
+      <c r="D8">
+        <v>21.6</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>22.5</v>
+      </c>
+      <c r="C9">
+        <v>22.7</v>
+      </c>
+      <c r="D9">
+        <v>21.6</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>22.5</v>
+      </c>
+      <c r="C10">
+        <v>22.6</v>
+      </c>
+      <c r="D10">
+        <v>21.6</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>22.5</v>
+      </c>
+      <c r="C11">
+        <v>22.6</v>
+      </c>
+      <c r="D11">
+        <v>21.6</v>
+      </c>
+      <c r="E11">
+        <v>22</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>22.5</v>
+      </c>
+      <c r="C12">
+        <v>22.6</v>
+      </c>
+      <c r="D12">
+        <v>21.6</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>22.5</v>
+      </c>
+      <c r="C13">
+        <v>22.6</v>
+      </c>
+      <c r="D13">
+        <v>21.6</v>
+      </c>
+      <c r="E13">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>22.5</v>
+      </c>
+      <c r="C14">
+        <v>22.6</v>
+      </c>
+      <c r="D14">
+        <v>21.6</v>
+      </c>
+      <c r="E14">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>22.5</v>
+      </c>
+      <c r="C15">
+        <v>22.7</v>
+      </c>
+      <c r="D15">
+        <v>21.6</v>
+      </c>
+      <c r="E15">
+        <v>22</v>
+      </c>
+      <c r="F15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>22.5</v>
+      </c>
+      <c r="C16">
+        <v>22.6</v>
+      </c>
+      <c r="D16">
+        <v>21.6</v>
+      </c>
+      <c r="E16">
+        <v>22</v>
+      </c>
+      <c r="F16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>22.5</v>
+      </c>
+      <c r="C17">
+        <v>22.6</v>
+      </c>
+      <c r="D17">
+        <v>21.6</v>
+      </c>
+      <c r="E17">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>22.5</v>
+      </c>
+      <c r="C18">
+        <v>22.7</v>
+      </c>
+      <c r="D18">
+        <v>21.6</v>
+      </c>
+      <c r="E18">
+        <v>22</v>
+      </c>
+      <c r="F18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>22.5</v>
+      </c>
+      <c r="C19">
+        <v>22.6</v>
+      </c>
+      <c r="D19">
+        <v>21.6</v>
+      </c>
+      <c r="E19">
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>22.5</v>
+      </c>
+      <c r="C20">
+        <v>22.6</v>
+      </c>
+      <c r="D20">
+        <v>21.6</v>
+      </c>
+      <c r="E20">
+        <v>22</v>
+      </c>
+      <c r="F20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>22.5</v>
+      </c>
+      <c r="C21">
+        <v>22.6</v>
+      </c>
+      <c r="D21">
+        <v>21.6</v>
+      </c>
+      <c r="E21">
+        <v>22</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>22.5</v>
+      </c>
+      <c r="C22">
+        <v>22.6</v>
+      </c>
+      <c r="D22">
+        <v>21.6</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>22.5</v>
+      </c>
+      <c r="C23">
+        <v>22.6</v>
+      </c>
+      <c r="D23">
+        <v>21.6</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>22.5</v>
+      </c>
+      <c r="C24">
+        <v>22.6</v>
+      </c>
+      <c r="D24">
+        <v>21.6</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>22.5</v>
+      </c>
+      <c r="C25">
+        <v>22.6</v>
+      </c>
+      <c r="D25">
+        <v>21.6</v>
+      </c>
+      <c r="E25">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>22.5</v>
+      </c>
+      <c r="C26">
+        <v>22.6</v>
+      </c>
+      <c r="D26">
+        <v>21.6</v>
+      </c>
+      <c r="E26">
+        <v>22</v>
+      </c>
+      <c r="F26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>22.5</v>
+      </c>
+      <c r="C27">
+        <v>22.6</v>
+      </c>
+      <c r="D27">
+        <v>21.6</v>
+      </c>
+      <c r="E27">
+        <v>22</v>
+      </c>
+      <c r="F27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>22.5</v>
+      </c>
+      <c r="C28">
+        <v>22.7</v>
+      </c>
+      <c r="D28">
+        <v>21.6</v>
+      </c>
+      <c r="E28">
+        <v>22</v>
+      </c>
+      <c r="F28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>22.5</v>
+      </c>
+      <c r="C29">
+        <v>22.6</v>
+      </c>
+      <c r="D29">
+        <v>21.6</v>
+      </c>
+      <c r="E29">
+        <v>22</v>
+      </c>
+      <c r="F29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>22.5</v>
+      </c>
+      <c r="C30">
+        <v>22.6</v>
+      </c>
+      <c r="D30">
+        <v>21.6</v>
+      </c>
+      <c r="E30">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>22.5</v>
+      </c>
+      <c r="C31">
+        <v>22.6</v>
+      </c>
+      <c r="D31">
+        <v>21.6</v>
+      </c>
+      <c r="E31">
+        <v>22</v>
+      </c>
+      <c r="F31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>22.5</v>
+      </c>
+      <c r="C32">
+        <v>22.6</v>
+      </c>
+      <c r="D32">
+        <v>21.6</v>
+      </c>
+      <c r="E32">
+        <v>22</v>
+      </c>
+      <c r="F32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>31.1</v>
+      </c>
+      <c r="B33">
+        <v>22.5</v>
+      </c>
+      <c r="C33">
+        <v>22.6</v>
+      </c>
+      <c r="D33">
+        <v>21.6</v>
+      </c>
+      <c r="E33">
+        <v>22</v>
+      </c>
+      <c r="F33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>32.1</v>
+      </c>
+      <c r="B34">
+        <v>22.5</v>
+      </c>
+      <c r="C34">
+        <v>22.7</v>
+      </c>
+      <c r="D34">
+        <v>21.6</v>
+      </c>
+      <c r="E34">
+        <v>22</v>
+      </c>
+      <c r="F34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>33.1</v>
+      </c>
+      <c r="B35">
+        <v>22.5</v>
+      </c>
+      <c r="C35">
+        <v>22.7</v>
+      </c>
+      <c r="D35">
+        <v>21.6</v>
+      </c>
+      <c r="E35">
+        <v>22</v>
+      </c>
+      <c r="F35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>34.1</v>
+      </c>
+      <c r="B36">
+        <v>22.5</v>
+      </c>
+      <c r="C36">
+        <v>22.6</v>
+      </c>
+      <c r="D36">
+        <v>21.6</v>
+      </c>
+      <c r="E36">
+        <v>22</v>
+      </c>
+      <c r="F36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>35.1</v>
+      </c>
+      <c r="B37">
+        <v>22.5</v>
+      </c>
+      <c r="C37">
+        <v>22.6</v>
+      </c>
+      <c r="D37">
+        <v>21.6</v>
+      </c>
+      <c r="E37">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>36.1</v>
+      </c>
+      <c r="B38">
+        <v>22.5</v>
+      </c>
+      <c r="C38">
+        <v>22.6</v>
+      </c>
+      <c r="D38">
+        <v>21.6</v>
+      </c>
+      <c r="E38">
+        <v>22</v>
+      </c>
+      <c r="F38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>37.1</v>
+      </c>
+      <c r="B39">
+        <v>22.5</v>
+      </c>
+      <c r="C39">
+        <v>22.6</v>
+      </c>
+      <c r="D39">
+        <v>21.6</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>38.1</v>
+      </c>
+      <c r="B40">
+        <v>22.5</v>
+      </c>
+      <c r="C40">
+        <v>22.6</v>
+      </c>
+      <c r="D40">
+        <v>21.6</v>
+      </c>
+      <c r="E40">
+        <v>22</v>
+      </c>
+      <c r="F40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>39.1</v>
+      </c>
+      <c r="B41">
+        <v>22.5</v>
+      </c>
+      <c r="C41">
+        <v>22.6</v>
+      </c>
+      <c r="D41">
+        <v>21.6</v>
+      </c>
+      <c r="E41">
+        <v>22</v>
+      </c>
+      <c r="F41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>40.1</v>
+      </c>
+      <c r="B42">
+        <v>22.4</v>
+      </c>
+      <c r="C42">
+        <v>22.6</v>
+      </c>
+      <c r="D42">
+        <v>21.6</v>
+      </c>
+      <c r="E42">
+        <v>22</v>
+      </c>
+      <c r="F42">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>41.1</v>
+      </c>
+      <c r="B43">
+        <v>22.4</v>
+      </c>
+      <c r="C43">
+        <v>22.6</v>
+      </c>
+      <c r="D43">
+        <v>21.6</v>
+      </c>
+      <c r="E43">
+        <v>22</v>
+      </c>
+      <c r="F43">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>42.1</v>
+      </c>
+      <c r="B44">
+        <v>22.4</v>
+      </c>
+      <c r="C44">
+        <v>22.6</v>
+      </c>
+      <c r="D44">
+        <v>21.6</v>
+      </c>
+      <c r="E44">
+        <v>22</v>
+      </c>
+      <c r="F44">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>43.1</v>
+      </c>
+      <c r="B45">
+        <v>22.4</v>
+      </c>
+      <c r="C45">
+        <v>22.6</v>
+      </c>
+      <c r="D45">
+        <v>21.6</v>
+      </c>
+      <c r="E45">
+        <v>22</v>
+      </c>
+      <c r="F45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>44.2</v>
+      </c>
+      <c r="B46">
+        <v>22.4</v>
+      </c>
+      <c r="C46">
+        <v>22.6</v>
+      </c>
+      <c r="D46">
+        <v>21.6</v>
+      </c>
+      <c r="E46">
+        <v>22</v>
+      </c>
+      <c r="F46">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>45.2</v>
+      </c>
+      <c r="B47">
+        <v>22.4</v>
+      </c>
+      <c r="C47">
+        <v>22.6</v>
+      </c>
+      <c r="D47">
+        <v>21.6</v>
+      </c>
+      <c r="E47">
+        <v>22</v>
+      </c>
+      <c r="F47">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>46.2</v>
+      </c>
+      <c r="B48">
+        <v>22.4</v>
+      </c>
+      <c r="C48">
+        <v>22.6</v>
+      </c>
+      <c r="D48">
+        <v>21.6</v>
+      </c>
+      <c r="E48">
+        <v>22</v>
+      </c>
+      <c r="F48">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>47.2</v>
+      </c>
+      <c r="B49">
+        <v>22.4</v>
+      </c>
+      <c r="C49">
+        <v>22.6</v>
+      </c>
+      <c r="D49">
+        <v>21.6</v>
+      </c>
+      <c r="E49">
+        <v>22</v>
+      </c>
+      <c r="F49">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>48.2</v>
+      </c>
+      <c r="B50">
+        <v>22.4</v>
+      </c>
+      <c r="C50">
+        <v>22.6</v>
+      </c>
+      <c r="D50">
+        <v>21.6</v>
+      </c>
+      <c r="E50">
+        <v>22</v>
+      </c>
+      <c r="F50">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>49.2</v>
+      </c>
+      <c r="B51">
+        <v>22.4</v>
+      </c>
+      <c r="C51">
+        <v>22.6</v>
+      </c>
+      <c r="D51">
+        <v>21.6</v>
+      </c>
+      <c r="E51">
+        <v>22</v>
+      </c>
+      <c r="F51">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>50.2</v>
+      </c>
+      <c r="B52">
+        <v>22.4</v>
+      </c>
+      <c r="C52">
+        <v>22.6</v>
+      </c>
+      <c r="D52">
+        <v>21.6</v>
+      </c>
+      <c r="E52">
+        <v>22</v>
+      </c>
+      <c r="F52">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>51.2</v>
+      </c>
+      <c r="B53">
+        <v>22.4</v>
+      </c>
+      <c r="C53">
+        <v>22.6</v>
+      </c>
+      <c r="D53">
+        <v>21.6</v>
+      </c>
+      <c r="E53">
+        <v>22</v>
+      </c>
+      <c r="F53">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>52.2</v>
+      </c>
+      <c r="B54">
+        <v>22.4</v>
+      </c>
+      <c r="C54">
+        <v>22.6</v>
+      </c>
+      <c r="D54">
+        <v>21.6</v>
+      </c>
+      <c r="E54">
+        <v>22</v>
+      </c>
+      <c r="F54">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>53.2</v>
+      </c>
+      <c r="B55">
+        <v>22.4</v>
+      </c>
+      <c r="C55">
+        <v>22.6</v>
+      </c>
+      <c r="D55">
+        <v>21.6</v>
+      </c>
+      <c r="E55">
+        <v>22</v>
+      </c>
+      <c r="F55">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>54.2</v>
+      </c>
+      <c r="B56">
+        <v>22.4</v>
+      </c>
+      <c r="C56">
+        <v>22.6</v>
+      </c>
+      <c r="D56">
+        <v>21.6</v>
+      </c>
+      <c r="E56">
+        <v>22</v>
+      </c>
+      <c r="F56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>55.2</v>
+      </c>
+      <c r="B57">
+        <v>22.4</v>
+      </c>
+      <c r="C57">
+        <v>22.6</v>
+      </c>
+      <c r="D57">
+        <v>21.6</v>
+      </c>
+      <c r="E57">
+        <v>22</v>
+      </c>
+      <c r="F57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>56.2</v>
+      </c>
+      <c r="B58">
+        <v>22.4</v>
+      </c>
+      <c r="C58">
+        <v>22.6</v>
+      </c>
+      <c r="D58">
+        <v>21.6</v>
+      </c>
+      <c r="E58">
+        <v>22</v>
+      </c>
+      <c r="F58">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>57.2</v>
+      </c>
+      <c r="B59">
+        <v>22.4</v>
+      </c>
+      <c r="C59">
+        <v>22.6</v>
+      </c>
+      <c r="D59">
+        <v>21.6</v>
+      </c>
+      <c r="E59">
+        <v>22</v>
+      </c>
+      <c r="F59">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>58.2</v>
+      </c>
+      <c r="B60">
+        <v>22.4</v>
+      </c>
+      <c r="C60">
+        <v>22.6</v>
+      </c>
+      <c r="D60">
+        <v>21.6</v>
+      </c>
+      <c r="E60">
+        <v>22</v>
+      </c>
+      <c r="F60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>59.2</v>
+      </c>
+      <c r="B61">
+        <v>22.4</v>
+      </c>
+      <c r="C61">
+        <v>22.6</v>
+      </c>
+      <c r="D61">
+        <v>21.6</v>
+      </c>
+      <c r="E61">
+        <v>22</v>
+      </c>
+      <c r="F61">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>60.2</v>
+      </c>
+      <c r="B62">
+        <v>22.4</v>
+      </c>
+      <c r="C62">
+        <v>22.6</v>
+      </c>
+      <c r="D62">
+        <v>21.6</v>
+      </c>
+      <c r="E62">
+        <v>22</v>
+      </c>
+      <c r="F62">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>61.2</v>
+      </c>
+      <c r="B63">
+        <v>22.4</v>
+      </c>
+      <c r="C63">
+        <v>22.6</v>
+      </c>
+      <c r="D63">
+        <v>21.6</v>
+      </c>
+      <c r="E63">
+        <v>22</v>
+      </c>
+      <c r="F63">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>62.2</v>
+      </c>
+      <c r="B64">
+        <v>22.4</v>
+      </c>
+      <c r="C64">
+        <v>22.6</v>
+      </c>
+      <c r="D64">
+        <v>21.6</v>
+      </c>
+      <c r="E64">
+        <v>22</v>
+      </c>
+      <c r="F64">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>63.2</v>
+      </c>
+      <c r="B65">
+        <v>22.4</v>
+      </c>
+      <c r="C65">
+        <v>22.6</v>
+      </c>
+      <c r="D65">
+        <v>21.6</v>
+      </c>
+      <c r="E65">
+        <v>22</v>
+      </c>
+      <c r="F65">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>64.2</v>
+      </c>
+      <c r="B66">
+        <v>22.4</v>
+      </c>
+      <c r="C66">
+        <v>22.6</v>
+      </c>
+      <c r="D66">
+        <v>21.6</v>
+      </c>
+      <c r="E66">
+        <v>22</v>
+      </c>
+      <c r="F66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>65.2</v>
+      </c>
+      <c r="B67">
+        <v>22.4</v>
+      </c>
+      <c r="C67">
+        <v>22.6</v>
+      </c>
+      <c r="D67">
+        <v>21.6</v>
+      </c>
+      <c r="E67">
+        <v>22</v>
+      </c>
+      <c r="F67">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>66.2</v>
+      </c>
+      <c r="B68">
+        <v>22.4</v>
+      </c>
+      <c r="C68">
+        <v>22.6</v>
+      </c>
+      <c r="D68">
+        <v>21.6</v>
+      </c>
+      <c r="E68">
+        <v>22</v>
+      </c>
+      <c r="F68">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>67.2</v>
+      </c>
+      <c r="B69">
+        <v>22.4</v>
+      </c>
+      <c r="C69">
+        <v>22.6</v>
+      </c>
+      <c r="D69">
+        <v>21.6</v>
+      </c>
+      <c r="E69">
+        <v>22</v>
+      </c>
+      <c r="F69">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <v>68.2</v>
+      </c>
+      <c r="B70">
+        <v>22.4</v>
+      </c>
+      <c r="C70">
+        <v>22.6</v>
+      </c>
+      <c r="D70">
+        <v>21.6</v>
+      </c>
+      <c r="E70">
+        <v>22</v>
+      </c>
+      <c r="F70">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>69.2</v>
+      </c>
+      <c r="B71">
+        <v>22.4</v>
+      </c>
+      <c r="C71">
+        <v>22.6</v>
+      </c>
+      <c r="D71">
+        <v>21.6</v>
+      </c>
+      <c r="E71">
+        <v>22</v>
+      </c>
+      <c r="F71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>70.2</v>
+      </c>
+      <c r="B72">
+        <v>22.4</v>
+      </c>
+      <c r="C72">
+        <v>22.6</v>
+      </c>
+      <c r="D72">
+        <v>21.6</v>
+      </c>
+      <c r="E72">
+        <v>22</v>
+      </c>
+      <c r="F72">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>71.2</v>
+      </c>
+      <c r="B73">
+        <v>22.4</v>
+      </c>
+      <c r="C73">
+        <v>22.6</v>
+      </c>
+      <c r="D73">
+        <v>21.6</v>
+      </c>
+      <c r="E73">
+        <v>22</v>
+      </c>
+      <c r="F73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>72.2</v>
+      </c>
+      <c r="B74">
+        <v>22.4</v>
+      </c>
+      <c r="C74">
+        <v>22.6</v>
+      </c>
+      <c r="D74">
+        <v>21.6</v>
+      </c>
+      <c r="E74">
+        <v>22</v>
+      </c>
+      <c r="F74">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>73.2</v>
+      </c>
+      <c r="B75">
+        <v>22.4</v>
+      </c>
+      <c r="C75">
+        <v>22.6</v>
+      </c>
+      <c r="D75">
+        <v>21.6</v>
+      </c>
+      <c r="E75">
+        <v>22</v>
+      </c>
+      <c r="F75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>74.2</v>
+      </c>
+      <c r="B76">
+        <v>22.4</v>
+      </c>
+      <c r="C76">
+        <v>22.6</v>
+      </c>
+      <c r="D76">
+        <v>21.6</v>
+      </c>
+      <c r="E76">
+        <v>22</v>
+      </c>
+      <c r="F76">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>75.2</v>
+      </c>
+      <c r="B77">
+        <v>22.4</v>
+      </c>
+      <c r="C77">
+        <v>22.6</v>
+      </c>
+      <c r="D77">
+        <v>21.6</v>
+      </c>
+      <c r="E77">
+        <v>22</v>
+      </c>
+      <c r="F77">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>76.2</v>
+      </c>
+      <c r="B78">
+        <v>22.4</v>
+      </c>
+      <c r="C78">
+        <v>22.6</v>
+      </c>
+      <c r="D78">
+        <v>21.6</v>
+      </c>
+      <c r="E78">
+        <v>22</v>
+      </c>
+      <c r="F78">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
+        <v>77.2</v>
+      </c>
+      <c r="B79">
+        <v>22.4</v>
+      </c>
+      <c r="C79">
+        <v>22.6</v>
+      </c>
+      <c r="D79">
+        <v>21.6</v>
+      </c>
+      <c r="E79">
+        <v>22</v>
+      </c>
+      <c r="F79">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <v>78.2</v>
+      </c>
+      <c r="B80">
+        <v>22.4</v>
+      </c>
+      <c r="C80">
+        <v>22.6</v>
+      </c>
+      <c r="D80">
+        <v>21.6</v>
+      </c>
+      <c r="E80">
+        <v>22</v>
+      </c>
+      <c r="F80">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <v>79.2</v>
+      </c>
+      <c r="B81">
+        <v>22.4</v>
+      </c>
+      <c r="C81">
+        <v>22.6</v>
+      </c>
+      <c r="D81">
+        <v>21.6</v>
+      </c>
+      <c r="E81">
+        <v>22</v>
+      </c>
+      <c r="F81">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>80.2</v>
+      </c>
+      <c r="B82">
+        <v>22.4</v>
+      </c>
+      <c r="C82">
+        <v>22.6</v>
+      </c>
+      <c r="D82">
+        <v>21.6</v>
+      </c>
+      <c r="E82">
+        <v>22</v>
+      </c>
+      <c r="F82">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>81.2</v>
+      </c>
+      <c r="B83">
+        <v>22.4</v>
+      </c>
+      <c r="C83">
+        <v>22.6</v>
+      </c>
+      <c r="D83">
+        <v>21.6</v>
+      </c>
+      <c r="E83">
+        <v>22</v>
+      </c>
+      <c r="F83">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>82.2</v>
+      </c>
+      <c r="B84">
+        <v>22.4</v>
+      </c>
+      <c r="C84">
+        <v>22.6</v>
+      </c>
+      <c r="D84">
+        <v>21.6</v>
+      </c>
+      <c r="E84">
+        <v>22</v>
+      </c>
+      <c r="F84">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <v>83.2</v>
+      </c>
+      <c r="B85">
+        <v>22.4</v>
+      </c>
+      <c r="C85">
+        <v>22.6</v>
+      </c>
+      <c r="D85">
+        <v>21.6</v>
+      </c>
+      <c r="E85">
+        <v>22</v>
+      </c>
+      <c r="F85">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>84.2</v>
+      </c>
+      <c r="B86">
+        <v>22.4</v>
+      </c>
+      <c r="C86">
+        <v>22.6</v>
+      </c>
+      <c r="D86">
+        <v>21.6</v>
+      </c>
+      <c r="E86">
+        <v>22</v>
+      </c>
+      <c r="F86">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <v>85.2</v>
+      </c>
+      <c r="B87">
+        <v>22.4</v>
+      </c>
+      <c r="C87">
+        <v>22.6</v>
+      </c>
+      <c r="D87">
+        <v>21.6</v>
+      </c>
+      <c r="E87">
+        <v>22</v>
+      </c>
+      <c r="F87">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>86.2</v>
+      </c>
+      <c r="B88">
+        <v>22.4</v>
+      </c>
+      <c r="C88">
+        <v>22.6</v>
+      </c>
+      <c r="D88">
+        <v>21.6</v>
+      </c>
+      <c r="E88">
+        <v>22</v>
+      </c>
+      <c r="F88">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V22 - Fixed graphical bugs, added option in menu to option data save path, fixed bug that prevented data from being properly saved
</commit_message>
<xml_diff>
--- a/MCC-DAQ backup/temp.xlsx
+++ b/MCC-DAQ backup/temp.xlsx
@@ -392,19 +392,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="nan" customWidth="1"/>
-    <col min="2" max="2" width="nan" customWidth="1"/>
-    <col min="3" max="3" width="nan" customWidth="1"/>
-    <col min="4" max="4" width="nan" customWidth="1"/>
-    <col min="5" max="5" width="nan" customWidth="1"/>
-    <col min="6" max="6" width="nan" customWidth="1"/>
-    <col min="7" max="7" width="nan" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -430,6 +430,98 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>26.9</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>25.4</v>
+      </c>
+      <c r="E2">
+        <v>25.3</v>
+      </c>
+      <c r="F2">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>26.9</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>25.4</v>
+      </c>
+      <c r="E3">
+        <v>25.3</v>
+      </c>
+      <c r="F3">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>26.9</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>25.4</v>
+      </c>
+      <c r="E4">
+        <v>25.3</v>
+      </c>
+      <c r="F4">
+        <v>99.2</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>26.9</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>25.4</v>
+      </c>
+      <c r="E5">
+        <v>25.4</v>
+      </c>
+      <c r="F5">
+        <v>99</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>